<commit_message>
Correção dos script, treinamento do modelo e preenchimento da planilha
</commit_message>
<xml_diff>
--- a/homologation.xlsx
+++ b/homologation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>Text</t>
   </si>
@@ -37,12 +37,18 @@
     <t>0.5015215873718262</t>
   </si>
   <si>
+    <t>1.0000100135803223</t>
+  </si>
+  <si>
     <t>This ruined my life</t>
   </si>
   <si>
     <t>0.5110940337181091</t>
   </si>
   <si>
+    <t>1.0000089406967163</t>
+  </si>
+  <si>
     <t>The smell is the worst part</t>
   </si>
   <si>
@@ -55,12 +61,18 @@
     <t>0.5046359300613403</t>
   </si>
   <si>
+    <t>1.0000035762786865</t>
+  </si>
+  <si>
     <t>Would recommend if it wasn't so overpriced</t>
   </si>
   <si>
     <t>0.5007198452949524</t>
   </si>
   <si>
+    <t>0.9997366070747375</t>
+  </si>
+  <si>
     <t>Such a great experience</t>
   </si>
   <si>
@@ -70,28 +82,43 @@
     <t>0.5139934420585632</t>
   </si>
   <si>
+    <t>0.9995201826095581</t>
+  </si>
+  <si>
     <t>Everyone should watch this</t>
   </si>
   <si>
     <t>0.5037869811058044</t>
   </si>
   <si>
+    <t>0.9673290252685547</t>
+  </si>
+  <si>
     <t>I love to watch this movie again and again</t>
   </si>
   <si>
     <t>0.5004516243934631</t>
   </si>
   <si>
+    <t>0.96995609998703</t>
+  </si>
+  <si>
     <t>This could not have helped more</t>
   </si>
   <si>
     <t>0.5041288137435913</t>
   </si>
   <si>
+    <t>0.5667021870613098</t>
+  </si>
+  <si>
     <t>My mom  enjoys listening to it</t>
   </si>
   <si>
     <t>0.5003058314323425</t>
+  </si>
+  <si>
+    <t>0.999575674533844</t>
   </si>
 </sst>
 </file>
@@ -167,29 +194,26 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -408,17 +432,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -446,10 +470,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -697,12 +721,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -989,7 +1013,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1017,10 +1041,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1278,7 +1302,7 @@
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.3516" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85156" style="1" customWidth="1"/>
@@ -1296,7 +1320,7 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" ht="28.8" customHeight="1">
+    <row r="2" ht="13.55" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" t="s" s="3">
@@ -1316,115 +1340,135 @@
       <c r="C3" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" t="s" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s" s="6">
         <v>6</v>
       </c>
       <c r="C4" t="s" s="6">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s" s="6">
         <v>6</v>
       </c>
       <c r="C5" t="s" s="6">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s" s="6">
         <v>6</v>
       </c>
       <c r="C6" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s" s="6">
         <v>6</v>
       </c>
       <c r="C7" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" t="s" s="6">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="D8" t="s" s="6">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" t="s" s="6">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="D9" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s" s="6">
         <v>21</v>
       </c>
-      <c r="B10" t="s" s="6">
-        <v>17</v>
-      </c>
       <c r="C10" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="D10" t="s" s="6">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D11" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="D11" t="s" s="6">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="D12" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="D12" t="s" s="6">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>